<commit_message>
update coeffs and tests
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/CropStage/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/CropStage/FieldConfigs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\CropStage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AC5687-2DD0-4C6B-8AE7-6CFCE246EBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3A109-B833-47D3-B14B-CF0E4B2426E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D0D9F3F3-C1B3-4B79-AF5D-93A117BC34BF}"/>
   </bookViews>
@@ -656,7 +656,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>